<commit_message>
Added two more materials and introduced them in the program
</commit_message>
<xml_diff>
--- a/training material/sources.xlsx
+++ b/training material/sources.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban\Desktop\training material\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban\Desktop\github\CS-Project-V2\training material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE61CD1-C031-4D1C-A80A-811C8B541DB4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37DE49F-5ED7-4D97-9E9A-3E3BCFE27E4F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{E7EDEF38-2786-41BF-B68B-71803720CE39}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
   <si>
     <t>Topic</t>
   </si>
@@ -142,6 +142,24 @@
   </si>
   <si>
     <t>Container registry</t>
+  </si>
+  <si>
+    <t>Networking</t>
+  </si>
+  <si>
+    <t>All the subtopics</t>
+  </si>
+  <si>
+    <t>https://console.bluemix.net/catalog/?category=network</t>
+  </si>
+  <si>
+    <t>networking</t>
+  </si>
+  <si>
+    <t>storage</t>
+  </si>
+  <si>
+    <t>https://console.bluemix.net/catalog/?category=storage</t>
   </si>
 </sst>
 </file>
@@ -504,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61093C55-F156-4456-BBF5-F7E37DC4DA73}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,6 +760,34 @@
         <v>35</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C14" r:id="rId1" xr:uid="{7657AEC2-AD9D-4FCE-8514-A183BDBF899F}"/>

</xml_diff>

<commit_message>
Updated sources table to include all of the new materials
</commit_message>
<xml_diff>
--- a/training material/sources.xlsx
+++ b/training material/sources.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban\Desktop\github\CS-Project-V2\training material\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Study files\cs project\new\CS-Project-V2-master\CS-Project-V2-master\training material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37DE49F-5ED7-4D97-9E9A-3E3BCFE27E4F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{E7EDEF38-2786-41BF-B68B-71803720CE39}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
   <si>
     <t>Topic</t>
   </si>
@@ -160,12 +159,102 @@
   </si>
   <si>
     <t>https://console.bluemix.net/catalog/?category=storage</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>https://console.bluemix.net/catalog/?category=ai</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>Analytics</t>
+  </si>
+  <si>
+    <t>https://console.bluemix.net/catalog/?category=analytics</t>
+  </si>
+  <si>
+    <t>analytics</t>
+  </si>
+  <si>
+    <t>Databases</t>
+  </si>
+  <si>
+    <t>https://console.bluemix.net/catalog/?category=databases</t>
+  </si>
+  <si>
+    <t>databases</t>
+  </si>
+  <si>
+    <t>Developer tools</t>
+  </si>
+  <si>
+    <t>https://console.bluemix.net/catalog/?category=devops</t>
+  </si>
+  <si>
+    <t>developer-tools</t>
+  </si>
+  <si>
+    <t>Integration</t>
+  </si>
+  <si>
+    <t>Internet f things</t>
+  </si>
+  <si>
+    <t>Security and Identity</t>
+  </si>
+  <si>
+    <t>Starter kits</t>
+  </si>
+  <si>
+    <t>Web and mobile</t>
+  </si>
+  <si>
+    <t>Web and application</t>
+  </si>
+  <si>
+    <t>integration</t>
+  </si>
+  <si>
+    <t>IOT</t>
+  </si>
+  <si>
+    <t>security-identity</t>
+  </si>
+  <si>
+    <t>starterkits</t>
+  </si>
+  <si>
+    <t>web-mobile</t>
+  </si>
+  <si>
+    <t>web-application</t>
+  </si>
+  <si>
+    <t>https://console.bluemix.net/catalog/?category=integration</t>
+  </si>
+  <si>
+    <t>https://console.bluemix.net/catalog/?category=iot</t>
+  </si>
+  <si>
+    <t>https://console.bluemix.net/catalog/?category=security</t>
+  </si>
+  <si>
+    <t>https://console.bluemix.net/catalog/?category=starterkits</t>
+  </si>
+  <si>
+    <t>https://console.bluemix.net/catalog/?category=mobile</t>
+  </si>
+  <si>
+    <t>https://console.bluemix.net/catalog/?category=app_services</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -521,11 +610,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61093C55-F156-4456-BBF5-F7E37DC4DA73}">
-  <dimension ref="A1:D21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +622,7 @@
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
     <col min="3" max="3" width="86.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -788,11 +877,154 @@
         <v>41</v>
       </c>
     </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C14" r:id="rId1" xr:uid="{7657AEC2-AD9D-4FCE-8514-A183BDBF899F}"/>
+    <hyperlink ref="C14" r:id="rId1"/>
+    <hyperlink ref="C27" r:id="rId2"/>
+    <hyperlink ref="C33" r:id="rId3"/>
+    <hyperlink ref="C37" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the sources materials and the databases
</commit_message>
<xml_diff>
--- a/training material/sources.xlsx
+++ b/training material/sources.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>Topic</t>
   </si>
@@ -53,81 +53,6 @@
     <t>Compute</t>
   </si>
   <si>
-    <t>Kubernetes Service</t>
-  </si>
-  <si>
-    <t>Bare Metal Server</t>
-  </si>
-  <si>
-    <t>compute2</t>
-  </si>
-  <si>
-    <t>compute3</t>
-  </si>
-  <si>
-    <t>WebSphere Application Server</t>
-  </si>
-  <si>
-    <t>HPCaaS from Rescale</t>
-  </si>
-  <si>
-    <t>compute4</t>
-  </si>
-  <si>
-    <t>compute5</t>
-  </si>
-  <si>
-    <t>VMware Virtual Data Centers</t>
-  </si>
-  <si>
-    <t>compute6</t>
-  </si>
-  <si>
-    <t>IBM cloud private hosted</t>
-  </si>
-  <si>
-    <t>compute7</t>
-  </si>
-  <si>
-    <t>FortiGate Appliances</t>
-  </si>
-  <si>
-    <t>compute8</t>
-  </si>
-  <si>
-    <t>IBM cloud secure virtualization</t>
-  </si>
-  <si>
-    <t>compute9</t>
-  </si>
-  <si>
-    <t>IBM spectrum protect</t>
-  </si>
-  <si>
-    <t>compute10</t>
-  </si>
-  <si>
-    <t>Veeam and zerto</t>
-  </si>
-  <si>
-    <t>compute11</t>
-  </si>
-  <si>
-    <t>Vmware managed services</t>
-  </si>
-  <si>
-    <t>compute12</t>
-  </si>
-  <si>
-    <t>functions</t>
-  </si>
-  <si>
-    <t>compute13</t>
-  </si>
-  <si>
-    <t>Cloud foundry</t>
-  </si>
-  <si>
     <t>Containers</t>
   </si>
   <si>
@@ -135,12 +60,6 @@
   </si>
   <si>
     <t>https://console.bluemix.net/catalog/?category=containers</t>
-  </si>
-  <si>
-    <t>containers2</t>
-  </si>
-  <si>
-    <t>Container registry</t>
   </si>
   <si>
     <t>Networking</t>
@@ -611,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +563,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -653,378 +572,195 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>32</v>
       </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" t="s">
         <v>39</v>
-      </c>
-      <c r="D19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>56</v>
-      </c>
-      <c r="B33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" t="s">
-        <v>69</v>
-      </c>
-      <c r="D35" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>58</v>
-      </c>
-      <c r="B37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>59</v>
-      </c>
-      <c r="B39" t="s">
-        <v>38</v>
-      </c>
-      <c r="C39" t="s">
-        <v>71</v>
-      </c>
-      <c r="D39" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>60</v>
-      </c>
-      <c r="B41" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" t="s">
-        <v>72</v>
-      </c>
-      <c r="D41" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C14" r:id="rId1"/>
-    <hyperlink ref="C27" r:id="rId2"/>
-    <hyperlink ref="C33" r:id="rId3"/>
-    <hyperlink ref="C37" r:id="rId4"/>
+    <hyperlink ref="C20" r:id="rId2"/>
+    <hyperlink ref="C24" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>